<commit_message>
Completed CRC check sum for GPS
</commit_message>
<xml_diff>
--- a/lib/mission127(PIP).xlsx
+++ b/lib/mission127(PIP).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Programming\vortex_parser\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41FD90C-0D5E-4E86-9356-CAD7BB4D9F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29DF972-ED7D-4D7C-ACEC-463917100DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
   <si>
     <t>Bitmask</t>
   </si>
@@ -50,9 +50,6 @@
     <t>mNLP</t>
   </si>
   <si>
-    <t>EFP</t>
-  </si>
-  <si>
     <t>ACC</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Count</t>
   </si>
   <si>
-    <t>FPP</t>
-  </si>
-  <si>
     <t>DIG ACC</t>
   </si>
   <si>
@@ -146,12 +140,6 @@
     <t>+3.3 V</t>
   </si>
   <si>
-    <t>House keeping:</t>
-  </si>
-  <si>
-    <t>End Row</t>
-  </si>
-  <si>
     <t>Start Row</t>
   </si>
   <si>
@@ -240,6 +228,30 @@
   </si>
   <si>
     <t>2d/3d</t>
+  </si>
+  <si>
+    <t>End Row (inc.)</t>
+  </si>
+  <si>
+    <t>Each unique window title cretes a window</t>
+  </si>
+  <si>
+    <t>Channels get assigned to the last created graph</t>
+  </si>
+  <si>
+    <t>Housekeeping:</t>
+  </si>
+  <si>
+    <t>Each row starts at column B and ends at first empty cell</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>(Dig. Acc is hard coded for ACC)</t>
+  </si>
+  <si>
+    <t>PIP</t>
   </si>
 </sst>
 </file>
@@ -372,7 +384,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -441,11 +453,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -522,6 +549,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7758D255-7225-412E-BCCB-5D6A66A51808}">
-  <dimension ref="A2:R47"/>
+  <dimension ref="A2:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,26 +889,26 @@
     <col min="2" max="22" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>11</v>
@@ -891,25 +919,31 @@
       <c r="F3" s="13">
         <v>4.96</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="32">
         <f>F3*5000*25</f>
         <v>620000</v>
       </c>
+      <c r="I3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4">
         <v>39</v>
       </c>
       <c r="D4">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C5">
         <v>45</v>
@@ -917,88 +951,91 @@
       <c r="D5">
         <v>47</v>
       </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="J9" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="14">
         <v>0</v>
       </c>
       <c r="F11" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>5</v>
       </c>
       <c r="H11" s="15">
         <v>5000</v>
@@ -1006,10 +1043,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12" s="11" t="b">
         <f>TRUE()</f>
@@ -1028,45 +1065,45 @@
         <v>255</v>
       </c>
       <c r="I12" s="9">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J12" s="9">
-        <v>240</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" s="11" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="E13" s="11">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F13" s="11">
         <v>255</v>
       </c>
       <c r="G13" s="10">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H13" s="10">
         <v>255</v>
       </c>
       <c r="I13" s="9">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J13" s="9">
-        <v>15</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>2</v>
@@ -1078,10 +1115,10 @@
         <v>1</v>
       </c>
       <c r="F15" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="15" t="s">
         <v>4</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>5</v>
       </c>
       <c r="H15" s="15">
         <v>5000</v>
@@ -1089,476 +1126,421 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="11">
+        <v>52</v>
+      </c>
+      <c r="F16" s="11">
+        <v>255</v>
+      </c>
+      <c r="G16" s="10">
+        <v>53</v>
+      </c>
+      <c r="H16" s="10">
+        <v>255</v>
+      </c>
+      <c r="I16" s="9">
+        <v>58</v>
+      </c>
+      <c r="J16" s="9">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C17" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="11">
+        <v>54</v>
+      </c>
+      <c r="F17" s="11">
+        <v>255</v>
+      </c>
+      <c r="G17" s="10">
+        <v>55</v>
+      </c>
+      <c r="H17" s="10">
+        <v>255</v>
+      </c>
+      <c r="I17" s="9">
+        <v>58</v>
+      </c>
+      <c r="J17" s="9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E16" s="11">
-        <v>36</v>
-      </c>
-      <c r="F16" s="11">
-        <v>255</v>
-      </c>
-      <c r="G16" s="10">
-        <v>37</v>
-      </c>
-      <c r="H16" s="10">
-        <v>255</v>
-      </c>
-      <c r="I16" s="9">
-        <v>39</v>
-      </c>
-      <c r="J16" s="9">
+      <c r="C18" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="11">
+        <v>56</v>
+      </c>
+      <c r="F18" s="11">
+        <v>255</v>
+      </c>
+      <c r="G18" s="10">
+        <v>57</v>
+      </c>
+      <c r="H18" s="10">
+        <v>255</v>
+      </c>
+      <c r="I18" s="9">
+        <v>58</v>
+      </c>
+      <c r="J18" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" s="14">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="15">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="11">
+        <v>59</v>
+      </c>
+      <c r="F21" s="11">
+        <v>255</v>
+      </c>
+      <c r="G21" s="10">
+        <v>60</v>
+      </c>
+      <c r="H21" s="10">
+        <v>255</v>
+      </c>
+      <c r="I21" s="9">
+        <v>63</v>
+      </c>
+      <c r="J21" s="9">
         <v>240</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="14" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E22" s="11">
+        <v>61</v>
+      </c>
+      <c r="F22" s="11">
+        <v>255</v>
+      </c>
+      <c r="G22" s="10">
+        <v>62</v>
+      </c>
+      <c r="H22" s="10">
+        <v>255</v>
+      </c>
+      <c r="I22" s="9">
+        <v>63</v>
+      </c>
+      <c r="J22" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E23" s="11">
+        <v>59</v>
+      </c>
+      <c r="F23" s="11">
+        <v>255</v>
+      </c>
+      <c r="G23" s="10">
+        <v>60</v>
+      </c>
+      <c r="H23" s="10">
+        <v>255</v>
+      </c>
+      <c r="I23" s="9">
+        <v>61</v>
+      </c>
+      <c r="J23" s="9">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="14">
+        <v>2</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="2">
-        <v>1</v>
-      </c>
-      <c r="E18" s="14">
-        <v>2</v>
-      </c>
-      <c r="F18" s="15" t="s">
+      <c r="G25" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="15">
+      <c r="H25" s="15">
         <v>5000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E19" s="11">
-        <v>52</v>
-      </c>
-      <c r="F19" s="11">
-        <v>255</v>
-      </c>
-      <c r="G19" s="10">
-        <v>53</v>
-      </c>
-      <c r="H19" s="10">
-        <v>255</v>
-      </c>
-      <c r="I19" s="9">
-        <v>58</v>
-      </c>
-      <c r="J19" s="9">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E20" s="11">
-        <v>54</v>
-      </c>
-      <c r="F20" s="11">
-        <v>255</v>
-      </c>
-      <c r="G20" s="10">
-        <v>55</v>
-      </c>
-      <c r="H20" s="10">
-        <v>255</v>
-      </c>
-      <c r="I20" s="9">
-        <v>58</v>
-      </c>
-      <c r="J20" s="9">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E21" s="11">
-        <v>56</v>
-      </c>
-      <c r="F21" s="11">
-        <v>255</v>
-      </c>
-      <c r="G21" s="10">
-        <v>57</v>
-      </c>
-      <c r="H21" s="10">
-        <v>255</v>
-      </c>
-      <c r="I21" s="9">
-        <v>58</v>
-      </c>
-      <c r="J21" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="2">
-        <v>2</v>
-      </c>
-      <c r="E23" s="14">
-        <v>1</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="15">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E24" s="11">
-        <v>59</v>
-      </c>
-      <c r="F24" s="11">
-        <v>255</v>
-      </c>
-      <c r="G24" s="10">
-        <v>60</v>
-      </c>
-      <c r="H24" s="10">
-        <v>255</v>
-      </c>
-      <c r="I24" s="9">
-        <v>63</v>
-      </c>
-      <c r="J24" s="9">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E25" s="11">
-        <v>61</v>
-      </c>
-      <c r="F25" s="11">
-        <v>255</v>
-      </c>
-      <c r="G25" s="10">
-        <v>62</v>
-      </c>
-      <c r="H25" s="10">
-        <v>255</v>
-      </c>
-      <c r="I25" s="9">
-        <v>63</v>
-      </c>
-      <c r="J25" s="9">
-        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="11">
         <v>12</v>
       </c>
-      <c r="C26" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E26" s="11">
-        <v>59</v>
-      </c>
       <c r="F26" s="11">
         <v>255</v>
       </c>
       <c r="G26" s="10">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="H26" s="10">
         <v>255</v>
       </c>
       <c r="I26" s="9">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="J26" s="9">
-        <v>240</v>
+        <v>255</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
+      <c r="B27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="11">
+        <v>15</v>
+      </c>
+      <c r="F27" s="11">
+        <v>255</v>
+      </c>
+      <c r="G27" s="10">
+        <v>16</v>
+      </c>
+      <c r="H27" s="10">
+        <v>255</v>
+      </c>
+      <c r="I27" s="9">
+        <v>17</v>
+      </c>
+      <c r="J27" s="9">
+        <v>255</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0</v>
-      </c>
-      <c r="E28" s="14">
+      <c r="B28" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E28" s="11">
+        <v>18</v>
+      </c>
+      <c r="F28" s="11">
+        <v>255</v>
+      </c>
+      <c r="G28" s="10">
+        <v>19</v>
+      </c>
+      <c r="H28" s="10">
+        <v>255</v>
+      </c>
+      <c r="I28" s="9">
+        <v>20</v>
+      </c>
+      <c r="J28" s="9">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+      <c r="E30" s="14">
         <v>2</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F30" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H28" s="15">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E29" s="11">
-        <v>12</v>
-      </c>
-      <c r="F29" s="11">
-        <v>255</v>
-      </c>
-      <c r="G29" s="10">
-        <v>13</v>
-      </c>
-      <c r="H29" s="10">
-        <v>255</v>
-      </c>
-      <c r="I29" s="9">
+      <c r="H30" s="15">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J29" s="9">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E30" s="11">
-        <v>15</v>
-      </c>
-      <c r="F30" s="11">
-        <v>255</v>
-      </c>
-      <c r="G30" s="10">
-        <v>16</v>
-      </c>
-      <c r="H30" s="10">
-        <v>255</v>
-      </c>
-      <c r="I30" s="9">
-        <v>17</v>
-      </c>
-      <c r="J30" s="9">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>10</v>
-      </c>
       <c r="D31" s="11" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E31" s="11">
-        <v>18</v>
-      </c>
-      <c r="F31" s="11">
-        <v>255</v>
-      </c>
-      <c r="G31" s="10">
-        <v>19</v>
-      </c>
-      <c r="H31" s="10">
-        <v>255</v>
-      </c>
-      <c r="I31" s="9">
-        <v>20</v>
-      </c>
-      <c r="J31" s="9">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1</v>
-      </c>
-      <c r="E33" s="14">
-        <v>2</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="15">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B34" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="11" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E31" s="11">
         <v>78</v>
       </c>
-      <c r="F34" s="11">
-        <v>255</v>
-      </c>
-      <c r="G34" s="9">
+      <c r="F31" s="11">
+        <v>255</v>
+      </c>
+      <c r="G31" s="9">
         <v>79</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H31" s="9">
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="11" t="b">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="11" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E32" s="11">
         <v>78</v>
       </c>
-      <c r="F35" s="11">
-        <v>255</v>
-      </c>
-      <c r="G35" s="9">
+      <c r="F32" s="11">
+        <v>255</v>
+      </c>
+      <c r="G32" s="9">
         <v>79</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H32" s="9">
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B38" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="27" t="s">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="29" t="s">
+      <c r="C39" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="F38" s="27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D39" s="2">
         <v>0</v>
@@ -1567,15 +1549,15 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D40" s="2">
         <v>1</v>
@@ -1584,111 +1566,94 @@
         <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1</v>
-      </c>
-      <c r="E41" s="2">
-        <v>1</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B44" s="30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C44" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="F44" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" s="21" t="s">
+      <c r="G44" s="22" t="s">
         <v>21</v>
-      </c>
-      <c r="G44" s="22" t="s">
-        <v>23</v>
       </c>
       <c r="H44" s="22" t="s">
         <v>0</v>
       </c>
       <c r="I44" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="J44" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="L44" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="K44" s="23" t="s">
+      <c r="M44" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="L44" s="23" t="s">
+      <c r="N44" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="M44" s="23" t="s">
+      <c r="O44" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="N44" s="24" t="s">
+      <c r="P44" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="O44" s="24" t="s">
+      <c r="Q44" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="R44" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="P44" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q44" s="24" t="s">
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="7">
         <v>33</v>
-      </c>
-      <c r="R44" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="7">
-        <v>131</v>
       </c>
       <c r="E45" s="7">
         <v>11</v>
       </c>
       <c r="F45" s="1">
-        <v>12500</v>
+        <v>50000</v>
       </c>
       <c r="G45" s="5">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H45" s="5">
-        <v>15</v>
+        <v>255</v>
       </c>
       <c r="I45" s="6" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="J45" s="6" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="K45" s="6" t="b">
         <f>FALSE()</f>
@@ -1723,12 +1688,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D46" s="26">
         <v>18</v>
@@ -1786,15 +1751,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D47" s="7">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="E47" s="7">
         <v>11</v>
@@ -1847,15 +1812,15 @@
       <c r="R47" s="6" t="b">
         <f>TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="T47" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="J46 M47" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1869,14 +1834,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085EDC4FCBFEAC44C90B472F1F1C900EA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e45273375250329c822a0a405177b348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xmlns:ns4="6b4e13fc-0909-4af8-88c8-1f82cb55b253" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0e1ca657407e685f067414fb59c7721" ns3:_="" ns4:_="">
     <xsd:import namespace="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
@@ -2105,6 +2062,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
   <ds:schemaRefs>
@@ -2114,23 +2079,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F39B334-7462-4EA1-A1AF-57733766443C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917E079B-BC71-4494-9E92-79C803C2F6BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2147,4 +2095,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F39B334-7462-4EA1-A1AF-57733766443C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjustments to excel format
</commit_message>
<xml_diff>
--- a/lib/mission127(PIP).xlsx
+++ b/lib/mission127(PIP).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Programming\vortex_parser\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290E7CD9-4089-443F-B7D9-FAB57BEC8727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04EA4DF-B12E-49FF-BAF9-028CFC7B71BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
   <si>
     <t>Bitmask</t>
   </si>
@@ -74,9 +74,6 @@
     <t>#3a749c</t>
   </si>
   <si>
-    <t>#deb110</t>
-  </si>
-  <si>
     <t>#de5510</t>
   </si>
   <si>
@@ -252,6 +249,12 @@
   </si>
   <si>
     <t>PIP</t>
+  </si>
+  <si>
+    <t>#7D2E8F</t>
+  </si>
+  <si>
+    <t>#78AB30</t>
   </si>
 </sst>
 </file>
@@ -280,7 +283,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +386,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7D2E8F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -472,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -555,6 +564,9 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -886,7 +898,7 @@
   <dimension ref="A2:T47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,19 +909,19 @@
   <sheetData>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>40</v>
-      </c>
       <c r="I2" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -930,12 +942,12 @@
         <v>620000</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>39</v>
@@ -944,12 +956,12 @@
         <v>40</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5">
         <v>45</v>
@@ -958,7 +970,7 @@
         <v>47</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -968,68 +980,68 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="G9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="J9" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -1079,7 +1091,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>8</v>
@@ -1109,7 +1121,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>2</v>
@@ -1162,7 +1174,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>8</v>
@@ -1192,7 +1204,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>8</v>
@@ -1222,7 +1234,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>5</v>
@@ -1248,7 +1260,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="11" t="b">
         <f>TRUE()</f>
@@ -1275,10 +1287,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>11</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>12</v>
       </c>
       <c r="D22" s="11" t="b">
         <f>TRUE()</f>
@@ -1304,11 +1316,11 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
-        <v>10</v>
+      <c r="B23" s="35" t="s">
+        <v>69</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="11" t="b">
         <f>TRUE()</f>
@@ -1335,7 +1347,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>1</v>
@@ -1390,7 +1402,7 @@
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>8</v>
@@ -1419,8 +1431,8 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="s">
-        <v>10</v>
+      <c r="B28" s="35" t="s">
+        <v>69</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>8</v>
@@ -1450,7 +1462,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>6</v>
@@ -1476,7 +1488,7 @@
         <v>9</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D31" s="11" t="b">
         <f>FALSE()</f>
@@ -1497,10 +1509,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32" s="11" t="b">
         <f>FALSE()</f>
@@ -1521,32 +1533,32 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B38" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="27" t="s">
         <v>60</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F38" s="27" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D39" s="2">
         <v>0</v>
@@ -1555,15 +1567,15 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D40" s="2">
         <v>1</v>
@@ -1572,68 +1584,68 @@
         <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="22" t="s">
         <v>20</v>
-      </c>
-      <c r="B44" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F44" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" s="22" t="s">
-        <v>21</v>
       </c>
       <c r="H44" s="22" t="s">
         <v>0</v>
       </c>
       <c r="I44" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J44" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="K44" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="K44" s="23" t="s">
+      <c r="L44" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="L44" s="23" t="s">
+      <c r="M44" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="M44" s="23" t="s">
+      <c r="N44" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="N44" s="24" t="s">
+      <c r="O44" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="O44" s="24" t="s">
+      <c r="P44" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="P44" s="24" t="s">
+      <c r="Q44" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="R44" s="23" t="s">
         <v>29</v>
-      </c>
-      <c r="Q44" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="R44" s="23" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C45" s="31" t="s">
         <v>8</v>
@@ -1764,7 +1776,7 @@
         <v>2</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D47" s="7">
         <v>51</v>
@@ -1822,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="T47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1833,11 +1845,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2070,27 +2083,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F39B334-7462-4EA1-A1AF-57733766443C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2115,9 +2118,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F39B334-7462-4EA1-A1AF-57733766443C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjusted to new parsing format
</commit_message>
<xml_diff>
--- a/lib/mission127(PIP).xlsx
+++ b/lib/mission127(PIP).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayash\Programming\vortex_parser\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04EA4DF-B12E-49FF-BAF9-028CFC7B71BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C26460D-2B58-49AD-BB1A-A2837C08B625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{93DD1A3E-79F5-40A0-9DE4-B4C0229D9C52}"/>
   </bookViews>
@@ -898,7 +898,7 @@
   <dimension ref="A2:T47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,6 +1854,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085EDC4FCBFEAC44C90B472F1F1C900EA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e45273375250329c822a0a405177b348">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xmlns:ns4="6b4e13fc-0909-4af8-88c8-1f82cb55b253" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0e1ca657407e685f067414fb59c7721" ns3:_="" ns4:_="">
     <xsd:import namespace="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
@@ -2082,14 +2090,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3be8e3c0-2842-4b5c-b060-a331e5ce9465" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B746C5C-9FCE-47B1-9B21-C70DB5E5E0E1}">
   <ds:schemaRefs>
@@ -2099,6 +2099,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F39B334-7462-4EA1-A1AF-57733766443C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{917E079B-BC71-4494-9E92-79C803C2F6BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2115,21 +2132,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F39B334-7462-4EA1-A1AF-57733766443C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3be8e3c0-2842-4b5c-b060-a331e5ce9465"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6b4e13fc-0909-4af8-88c8-1f82cb55b253"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>